<commit_message>
Added caches, logging and some other stuff
</commit_message>
<xml_diff>
--- a/2024_fantasy_constructor_data.xlsx
+++ b/2024_fantasy_constructor_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K231"/>
+  <dimension ref="A1:K241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8556,6 +8556,358 @@
         <v>23</v>
       </c>
     </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Alpine F1 Team</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>11</v>
+      </c>
+      <c r="C232" t="n">
+        <v>6</v>
+      </c>
+      <c r="D232" t="inlineStr"/>
+      <c r="E232" t="n">
+        <v>0</v>
+      </c>
+      <c r="F232" t="n">
+        <v>0</v>
+      </c>
+      <c r="G232" t="n">
+        <v>0</v>
+      </c>
+      <c r="H232" t="n">
+        <v>0</v>
+      </c>
+      <c r="I232" t="n">
+        <v>17</v>
+      </c>
+      <c r="J232" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K232" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Aston Martin</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>3</v>
+      </c>
+      <c r="C233" t="n">
+        <v>8</v>
+      </c>
+      <c r="D233" t="inlineStr"/>
+      <c r="E233" t="n">
+        <v>0</v>
+      </c>
+      <c r="F233" t="n">
+        <v>0</v>
+      </c>
+      <c r="G233" t="n">
+        <v>0</v>
+      </c>
+      <c r="H233" t="n">
+        <v>0</v>
+      </c>
+      <c r="I233" t="n">
+        <v>11</v>
+      </c>
+      <c r="J233" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K233" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Ferrari</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>58</v>
+      </c>
+      <c r="C234" t="n">
+        <v>8</v>
+      </c>
+      <c r="D234" t="inlineStr"/>
+      <c r="E234" t="n">
+        <v>0</v>
+      </c>
+      <c r="F234" t="n">
+        <v>0</v>
+      </c>
+      <c r="G234" t="n">
+        <v>0</v>
+      </c>
+      <c r="H234" t="n">
+        <v>0</v>
+      </c>
+      <c r="I234" t="n">
+        <v>66</v>
+      </c>
+      <c r="J234" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K234" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Haas F1 Team</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>18</v>
+      </c>
+      <c r="C235" t="n">
+        <v>8</v>
+      </c>
+      <c r="D235" t="n">
+        <v>-100.411</v>
+      </c>
+      <c r="E235" t="n">
+        <v>20</v>
+      </c>
+      <c r="F235" t="n">
+        <v>0</v>
+      </c>
+      <c r="G235" t="n">
+        <v>0</v>
+      </c>
+      <c r="H235" t="n">
+        <v>0</v>
+      </c>
+      <c r="I235" t="n">
+        <v>46</v>
+      </c>
+      <c r="J235" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K235" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>McLaren</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>37</v>
+      </c>
+      <c r="C236" t="n">
+        <v>13</v>
+      </c>
+      <c r="D236" t="inlineStr"/>
+      <c r="E236" t="n">
+        <v>0</v>
+      </c>
+      <c r="F236" t="n">
+        <v>0</v>
+      </c>
+      <c r="G236" t="n">
+        <v>0</v>
+      </c>
+      <c r="H236" t="n">
+        <v>0</v>
+      </c>
+      <c r="I236" t="n">
+        <v>50</v>
+      </c>
+      <c r="J236" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K236" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Mercedes</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>39</v>
+      </c>
+      <c r="C237" t="n">
+        <v>6</v>
+      </c>
+      <c r="D237" t="inlineStr"/>
+      <c r="E237" t="n">
+        <v>0</v>
+      </c>
+      <c r="F237" t="n">
+        <v>0</v>
+      </c>
+      <c r="G237" t="n">
+        <v>0</v>
+      </c>
+      <c r="H237" t="n">
+        <v>0</v>
+      </c>
+      <c r="I237" t="n">
+        <v>45</v>
+      </c>
+      <c r="J237" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K237" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>RB F1 Team</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>-6</v>
+      </c>
+      <c r="C238" t="n">
+        <v>3</v>
+      </c>
+      <c r="D238" t="inlineStr"/>
+      <c r="E238" t="n">
+        <v>0</v>
+      </c>
+      <c r="F238" t="n">
+        <v>0</v>
+      </c>
+      <c r="G238" t="n">
+        <v>0</v>
+      </c>
+      <c r="H238" t="n">
+        <v>0</v>
+      </c>
+      <c r="I238" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J238" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K238" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>13</v>
+      </c>
+      <c r="C239" t="n">
+        <v>13</v>
+      </c>
+      <c r="D239" t="inlineStr"/>
+      <c r="E239" t="n">
+        <v>0</v>
+      </c>
+      <c r="F239" t="n">
+        <v>0</v>
+      </c>
+      <c r="G239" t="n">
+        <v>0</v>
+      </c>
+      <c r="H239" t="n">
+        <v>0</v>
+      </c>
+      <c r="I239" t="n">
+        <v>26</v>
+      </c>
+      <c r="J239" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K239" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Sauber</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>-5</v>
+      </c>
+      <c r="C240" t="n">
+        <v>6</v>
+      </c>
+      <c r="D240" t="inlineStr"/>
+      <c r="E240" t="n">
+        <v>0</v>
+      </c>
+      <c r="F240" t="n">
+        <v>0</v>
+      </c>
+      <c r="G240" t="n">
+        <v>0</v>
+      </c>
+      <c r="H240" t="n">
+        <v>0</v>
+      </c>
+      <c r="I240" t="n">
+        <v>1</v>
+      </c>
+      <c r="J240" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K240" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>8</v>
+      </c>
+      <c r="C241" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D241" t="inlineStr"/>
+      <c r="E241" t="n">
+        <v>0</v>
+      </c>
+      <c r="F241" t="n">
+        <v>0</v>
+      </c>
+      <c r="G241" t="n">
+        <v>0</v>
+      </c>
+      <c r="H241" t="n">
+        <v>0</v>
+      </c>
+      <c r="I241" t="n">
+        <v>7</v>
+      </c>
+      <c r="J241" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K241" t="n">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>